<commit_message>
restructure and finish docs
</commit_message>
<xml_diff>
--- a/calculations/master_spreadsheet.xlsx
+++ b/calculations/master_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sucha\programming\offset_me\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957541A9-500C-420E-8E88-80C4FF82B01A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741B87E0-CDDA-4126-BE0F-8992433D5A39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1382,7 +1382,7 @@
   <dimension ref="A1:AJ52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>SUM(I2:ZZ2)</f>
+        <f t="shared" ref="A2:A14" si="0">SUM(I2:ZZ2)</f>
         <v>28</v>
       </c>
       <c r="B2" t="s">
@@ -1615,7 +1615,7 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>SUM(I3:ZZ3)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B3" t="s">
@@ -1729,7 +1729,7 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>SUM(I4:ZZ4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -1841,7 +1841,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>SUM(I5:ZZ5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B5" t="s">
@@ -1953,7 +1953,7 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>SUM(I6:ZZ6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B6" t="s">
@@ -2065,7 +2065,7 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>SUM(I7:ZZ7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B7" t="s">
@@ -2179,7 +2179,7 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>SUM(I8:ZZ8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B8" t="s">
@@ -2293,7 +2293,7 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>SUM(I9:ZZ9)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B9" t="s">
@@ -2408,7 +2408,7 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>SUM(I10:ZZ10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B10" t="s">
@@ -2522,7 +2522,7 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>SUM(I11:ZZ11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B11" t="s">
@@ -2636,7 +2636,7 @@
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>SUM(I12:ZZ12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B12" t="s">
@@ -2750,7 +2750,7 @@
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>SUM(I13:ZZ13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B13" t="s">
@@ -2864,7 +2864,7 @@
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>SUM(I14:ZZ14)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B14" t="s">
@@ -2878,11 +2878,11 @@
         <v>3.4141275690196928</v>
       </c>
       <c r="E14">
-        <f t="shared" ref="E14:F14" si="0">E15+E16+E17</f>
+        <f t="shared" ref="E14:F14" si="1">E15+E16+E17</f>
         <v>10.598492960684734</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47.372629840114826</v>
       </c>
       <c r="G14">
@@ -2979,7 +2979,7 @@
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" ref="A15:A16" si="1">SUM(I15:ZZ15)</f>
+        <f t="shared" ref="A15:A16" si="2">SUM(I15:ZZ15)</f>
         <v>1</v>
       </c>
       <c r="B15" t="s">
@@ -3093,7 +3093,7 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="B16" t="s">
@@ -3207,7 +3207,7 @@
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" ref="A17" si="2">SUM(I17:ZZ17)</f>
+        <f t="shared" ref="A17" si="3">SUM(I17:ZZ17)</f>
         <v>1</v>
       </c>
       <c r="B17" t="s">
@@ -3321,7 +3321,7 @@
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>SUM(I18:ZZ18)</f>
+        <f t="shared" ref="A18:A25" si="4">SUM(I18:ZZ18)</f>
         <v>28</v>
       </c>
       <c r="B18" t="s">
@@ -3436,7 +3436,7 @@
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>SUM(I19:ZZ19)</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="B19" t="s">
@@ -3547,7 +3547,7 @@
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>SUM(I20:ZZ20)</f>
+        <f t="shared" si="4"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="B20" t="s">
@@ -3658,7 +3658,7 @@
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>SUM(I21:ZZ21)</f>
+        <f t="shared" si="4"/>
         <v>1.0000000010000001</v>
       </c>
       <c r="B21" t="s">
@@ -3769,7 +3769,7 @@
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>SUM(I22:ZZ22)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="B22" t="s">
@@ -3880,7 +3880,7 @@
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>SUM(I23:ZZ23)</f>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="B23" t="s">
@@ -3891,18 +3891,19 @@
       </c>
       <c r="D23">
         <f>SUM(D24:D25)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <f>SUM(E24:E25)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23">
         <f>SUM(F24:F25)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G23">
-        <v>50</v>
+        <f>SUM(G24:G25)</f>
+        <v>30</v>
       </c>
       <c r="H23" t="s">
         <v>49</v>
@@ -3994,7 +3995,7 @@
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>SUM(I24:ZZ24)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="B24" t="s">
@@ -4004,16 +4005,16 @@
         <v>54</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H24" t="s">
         <v>49</v>
@@ -4105,7 +4106,7 @@
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>SUM(I25:ZZ25)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="B25" t="s">
@@ -4124,7 +4125,7 @@
         <v>10</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H25" t="s">
         <v>49</v>
@@ -4217,158 +4218,158 @@
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="E26">
         <f>(E23+E18+E2)/12</f>
-        <v>19.827713388023909</v>
+        <v>19.911046721357241</v>
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
-        <f>B1</f>
+        <f t="shared" ref="B28:AJ28" si="5">B1</f>
         <v>ID</v>
       </c>
       <c r="C28" t="str">
-        <f>C1</f>
+        <f t="shared" si="5"/>
         <v>Name</v>
       </c>
       <c r="D28" t="str">
-        <f>D1</f>
+        <f t="shared" si="5"/>
         <v>Low</v>
       </c>
       <c r="E28" t="str">
-        <f>E1</f>
+        <f t="shared" si="5"/>
         <v>Mid</v>
       </c>
       <c r="F28" t="str">
-        <f>F1</f>
+        <f t="shared" si="5"/>
         <v>High</v>
       </c>
       <c r="G28" t="str">
-        <f>G1</f>
+        <f t="shared" si="5"/>
         <v>Max</v>
       </c>
       <c r="H28" t="str">
-        <f>H1</f>
+        <f t="shared" si="5"/>
         <v>Unit</v>
       </c>
       <c r="I28" t="str">
-        <f>I1</f>
+        <f t="shared" si="5"/>
         <v>Malaria Consortium</v>
       </c>
       <c r="J28" t="str">
-        <f>J1</f>
+        <f t="shared" si="5"/>
         <v>Against Malaria Foundation</v>
       </c>
       <c r="K28" t="str">
-        <f>K1</f>
+        <f t="shared" si="5"/>
         <v>Deworm the World</v>
       </c>
       <c r="L28" t="str">
-        <f>L1</f>
+        <f t="shared" si="5"/>
         <v>Helen Keller International</v>
       </c>
       <c r="M28" t="str">
-        <f>M1</f>
+        <f t="shared" si="5"/>
         <v>New Incentives</v>
       </c>
       <c r="N28" t="str">
-        <f>N1</f>
+        <f t="shared" si="5"/>
         <v>GiveDirectly</v>
       </c>
       <c r="O28" t="str">
-        <f>O1</f>
+        <f t="shared" si="5"/>
         <v>The END Fund</v>
       </c>
       <c r="P28" t="str">
-        <f>P1</f>
+        <f t="shared" si="5"/>
         <v>SCI Foundation</v>
       </c>
       <c r="Q28" t="str">
-        <f>Q1</f>
+        <f t="shared" si="5"/>
         <v>Sightsavers</v>
       </c>
       <c r="R28" t="str">
-        <f>R1</f>
+        <f t="shared" si="5"/>
         <v>Village Enterprise</v>
       </c>
       <c r="S28" t="str">
-        <f>S1</f>
+        <f t="shared" si="5"/>
         <v>Seva</v>
       </c>
       <c r="T28" t="str">
-        <f>T1</f>
+        <f t="shared" si="5"/>
         <v>JAAGO Foundation</v>
       </c>
       <c r="U28" t="str">
-        <f>U1</f>
+        <f t="shared" si="5"/>
         <v>UNICEF south africa</v>
       </c>
       <c r="V28" t="str">
-        <f>V1</f>
+        <f t="shared" si="5"/>
         <v>Lola Karimova-Tillyaeva</v>
       </c>
       <c r="W28" t="str">
-        <f>W1</f>
+        <f t="shared" si="5"/>
         <v>Cambodian Children's Fund</v>
       </c>
       <c r="X28" t="str">
-        <f>X1</f>
+        <f t="shared" si="5"/>
         <v>Plan vivo</v>
       </c>
       <c r="Y28" t="str">
-        <f>Y1</f>
+        <f t="shared" si="5"/>
         <v>Gold Standard</v>
       </c>
       <c r="Z28" t="str">
-        <f>Z1</f>
+        <f t="shared" si="5"/>
         <v>Founders Pledge Climate change fund</v>
       </c>
       <c r="AA28" t="str">
-        <f>AA1</f>
+        <f t="shared" si="5"/>
         <v>Clean Air Task Force</v>
       </c>
       <c r="AB28" t="str">
-        <f>AB1</f>
+        <f t="shared" si="5"/>
         <v>WILD Foundation</v>
       </c>
       <c r="AC28" t="str">
-        <f>AC1</f>
+        <f t="shared" si="5"/>
         <v>Cool earth</v>
       </c>
       <c r="AD28" t="str">
-        <f>AD1</f>
+        <f t="shared" si="5"/>
         <v>ACE's Recommended Charity Fund</v>
       </c>
       <c r="AE28" t="str">
-        <f>AE1</f>
+        <f t="shared" si="5"/>
         <v>New Harvest</v>
       </c>
       <c r="AF28" t="str">
-        <f>AF1</f>
+        <f t="shared" si="5"/>
         <v>Oceana</v>
       </c>
       <c r="AG28" t="str">
-        <f>AG1</f>
+        <f t="shared" si="5"/>
         <v>Environmental Working Group</v>
       </c>
       <c r="AH28" t="str">
-        <f>AH1</f>
+        <f t="shared" si="5"/>
         <v>Rainforest alliance</v>
       </c>
       <c r="AI28" t="str">
-        <f>AI1</f>
+        <f t="shared" si="5"/>
         <v>Sustainable Food Trust</v>
       </c>
       <c r="AJ28" t="str">
-        <f>AJ1</f>
+        <f t="shared" si="5"/>
         <v>OceanCleanup</v>
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
-        <f>B2</f>
+        <f t="shared" ref="B29:C41" si="6">B2</f>
         <v>offset-planetary</v>
       </c>
       <c r="C29" t="str">
-        <f>C2</f>
+        <f t="shared" si="6"/>
         <v>Planetary boundaries</v>
       </c>
       <c r="D29">
@@ -4384,133 +4385,133 @@
         <v>32.336362688602421</v>
       </c>
       <c r="G29">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B2,1)))),100,ROUND(G2/12, 1 - _xlfn.CEILING.MATH(LOG10(G2/12))))</f>
+        <f t="shared" ref="G29:G52" si="7">IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B2,1)))),100,ROUND(G2/12, 1 - _xlfn.CEILING.MATH(LOG10(G2/12))))</f>
         <v>50</v>
       </c>
       <c r="H29" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B2,1))),"$","%")</f>
+        <f t="shared" ref="H29:H52" si="8">IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B2,1))),"$","%")</f>
         <v>$</v>
       </c>
       <c r="I29">
-        <f>IF($H29="%",I2/100,I2)</f>
+        <f t="shared" ref="I29:AJ29" si="9">IF($H29="%",I2/100,I2)</f>
         <v>1</v>
       </c>
       <c r="J29">
-        <f>IF($H29="%",J2/100,J2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K29">
-        <f>IF($H29="%",K2/100,K2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="L29">
-        <f>IF($H29="%",L2/100,L2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M29">
-        <f>IF($H29="%",M2/100,M2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="N29">
-        <f>IF($H29="%",N2/100,N2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O29">
-        <f>IF($H29="%",O2/100,O2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="P29">
-        <f>IF($H29="%",P2/100,P2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Q29">
-        <f>IF($H29="%",Q2/100,Q2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="R29">
-        <f>IF($H29="%",R2/100,R2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="S29">
-        <f>IF($H29="%",S2/100,S2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="T29">
-        <f>IF($H29="%",T2/100,T2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="U29">
-        <f>IF($H29="%",U2/100,U2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="V29">
-        <f>IF($H29="%",V2/100,V2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="W29">
-        <f>IF($H29="%",W2/100,W2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="X29">
-        <f>IF($H29="%",X2/100,X2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Y29">
-        <f>IF($H29="%",Y2/100,Y2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Z29">
-        <f>IF($H29="%",Z2/100,Z2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AA29">
-        <f>IF($H29="%",AA2/100,AA2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AB29">
-        <f>IF($H29="%",AB2/100,AB2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AC29">
-        <f>IF($H29="%",AC2/100,AC2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AD29">
-        <f>IF($H29="%",AD2/100,AD2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AE29">
-        <f>IF($H29="%",AE2/100,AE2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AF29">
-        <f>IF($H29="%",AF2/100,AF2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AG29">
-        <f>IF($H29="%",AG2/100,AG2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH29">
-        <f>IF($H29="%",AH2/100,AH2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AI29">
-        <f>IF($H29="%",AI2/100,AI2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AJ29">
-        <f>IF($H29="%",AJ2/100,AJ2)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
-        <f>B3</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary0</v>
       </c>
       <c r="C30" t="str">
-        <f>C3</f>
+        <f t="shared" si="6"/>
         <v>Climate crisis</v>
       </c>
       <c r="D30">
@@ -4526,1695 +4527,1695 @@
         <v>80.283905034269708</v>
       </c>
       <c r="G30">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B3,1)))),100,ROUND(G3/12, 1 - _xlfn.CEILING.MATH(LOG10(G3/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H30" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B3,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I30">
-        <f>IF($H30="%",I3/100,I3)</f>
+        <f t="shared" ref="I30:AJ30" si="10">IF($H30="%",I3/100,I3)</f>
         <v>0.01</v>
       </c>
       <c r="J30">
-        <f>IF($H30="%",J3/100,J3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="K30">
-        <f>IF($H30="%",K3/100,K3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="L30">
-        <f>IF($H30="%",L3/100,L3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="M30">
-        <f>IF($H30="%",M3/100,M3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="N30">
-        <f>IF($H30="%",N3/100,N3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="O30">
-        <f>IF($H30="%",O3/100,O3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="P30">
-        <f>IF($H30="%",P3/100,P3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="Q30">
-        <f>IF($H30="%",Q3/100,Q3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="R30">
-        <f>IF($H30="%",R3/100,R3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="S30">
-        <f>IF($H30="%",S3/100,S3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="T30">
-        <f>IF($H30="%",T3/100,T3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="U30">
-        <f>IF($H30="%",U3/100,U3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="V30">
-        <f>IF($H30="%",V3/100,V3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="W30">
-        <f>IF($H30="%",W3/100,W3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="X30">
-        <f>IF($H30="%",X3/100,X3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="Y30">
-        <f>IF($H30="%",Y3/100,Y3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="Z30">
-        <f>IF($H30="%",Z3/100,Z3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="AA30">
-        <f>IF($H30="%",AA3/100,AA3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="AB30">
-        <f>IF($H30="%",AB3/100,AB3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="AC30">
-        <f>IF($H30="%",AC3/100,AC3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="AD30">
-        <f>IF($H30="%",AD3/100,AD3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="AE30">
-        <f>IF($H30="%",AE3/100,AE3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="AF30">
-        <f>IF($H30="%",AF3/100,AF3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="AG30">
-        <f>IF($H30="%",AG3/100,AG3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="AH30">
-        <f>IF($H30="%",AH3/100,AH3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="AI30">
-        <f>IF($H30="%",AI3/100,AI3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
       <c r="AJ30">
-        <f>IF($H30="%",AJ3/100,AJ3)</f>
+        <f t="shared" si="10"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
-        <f>B4</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary00</v>
       </c>
       <c r="C31" t="str">
-        <f>C4</f>
+        <f t="shared" si="6"/>
         <v>Nature based offsets</v>
       </c>
       <c r="D31">
-        <f>IF($H4="%",D4*100,D4/12)</f>
+        <f t="shared" ref="D31:F33" si="11">IF($H4="%",D4*100,D4/12)</f>
         <v>0</v>
       </c>
       <c r="E31">
-        <f>IF($H4="%",E4*100,E4/12)</f>
+        <f t="shared" si="11"/>
         <v>33.333333333333329</v>
       </c>
       <c r="F31">
-        <f>IF($H4="%",F4*100,F4/12)</f>
+        <f t="shared" si="11"/>
         <v>100</v>
       </c>
       <c r="G31">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B4,1)))),100,ROUND(G4/12, 1 - _xlfn.CEILING.MATH(LOG10(G4/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H31" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B4,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I31">
-        <f>IF($H31="%",I4/100,I4)</f>
+        <f t="shared" ref="I31:AJ31" si="12">IF($H31="%",I4/100,I4)</f>
         <v>0</v>
       </c>
       <c r="J31">
-        <f>IF($H31="%",J4/100,J4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K31">
-        <f>IF($H31="%",K4/100,K4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L31">
-        <f>IF($H31="%",L4/100,L4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M31">
-        <f>IF($H31="%",M4/100,M4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N31">
-        <f>IF($H31="%",N4/100,N4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O31">
-        <f>IF($H31="%",O4/100,O4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P31">
-        <f>IF($H31="%",P4/100,P4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q31">
-        <f>IF($H31="%",Q4/100,Q4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="R31">
-        <f>IF($H31="%",R4/100,R4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S31">
-        <f>IF($H31="%",S4/100,S4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T31">
-        <f>IF($H31="%",T4/100,T4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U31">
-        <f>IF($H31="%",U4/100,U4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="V31">
-        <f>IF($H31="%",V4/100,V4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="W31">
-        <f>IF($H31="%",W4/100,W4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X31">
-        <f>IF($H31="%",X4/100,X4)</f>
+        <f t="shared" si="12"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="Y31">
-        <f>IF($H31="%",Y4/100,Y4)</f>
+        <f t="shared" si="12"/>
         <v>1E-3</v>
       </c>
       <c r="Z31">
-        <f>IF($H31="%",Z4/100,Z4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AA31">
-        <f>IF($H31="%",AA4/100,AA4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AB31">
-        <f>IF($H31="%",AB4/100,AB4)</f>
+        <f t="shared" si="12"/>
         <v>2E-3</v>
       </c>
       <c r="AC31">
-        <f>IF($H31="%",AC4/100,AC4)</f>
+        <f t="shared" si="12"/>
         <v>2E-3</v>
       </c>
       <c r="AD31">
-        <f>IF($H31="%",AD4/100,AD4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AE31">
-        <f>IF($H31="%",AE4/100,AE4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AF31">
-        <f>IF($H31="%",AF4/100,AF4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AG31">
-        <f>IF($H31="%",AG4/100,AG4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH31">
-        <f>IF($H31="%",AH4/100,AH4)</f>
+        <f t="shared" si="12"/>
         <v>2E-3</v>
       </c>
       <c r="AI31">
-        <f>IF($H31="%",AI4/100,AI4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AJ31">
-        <f>IF($H31="%",AJ4/100,AJ4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
-        <f>B5</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary01</v>
       </c>
       <c r="C32" t="str">
-        <f>C5</f>
+        <f t="shared" si="6"/>
         <v>Reducing emissions</v>
       </c>
       <c r="D32">
-        <f>IF($H5="%",D5*100,D5/12)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E32">
-        <f>IF($H5="%",E5*100,E5/12)</f>
+        <f t="shared" si="11"/>
         <v>33.333333333333329</v>
       </c>
       <c r="F32">
-        <f>IF($H5="%",F5*100,F5/12)</f>
+        <f t="shared" si="11"/>
         <v>100</v>
       </c>
       <c r="G32">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B5,1)))),100,ROUND(G5/12, 1 - _xlfn.CEILING.MATH(LOG10(G5/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H32" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B5,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I32">
-        <f>IF($H32="%",I5/100,I5)</f>
+        <f t="shared" ref="I32:AJ32" si="13">IF($H32="%",I5/100,I5)</f>
         <v>0</v>
       </c>
       <c r="J32">
-        <f>IF($H32="%",J5/100,J5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K32">
-        <f>IF($H32="%",K5/100,K5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L32">
-        <f>IF($H32="%",L5/100,L5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M32">
-        <f>IF($H32="%",M5/100,M5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="N32">
-        <f>IF($H32="%",N5/100,N5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="O32">
-        <f>IF($H32="%",O5/100,O5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P32">
-        <f>IF($H32="%",P5/100,P5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q32">
-        <f>IF($H32="%",Q5/100,Q5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="R32">
-        <f>IF($H32="%",R5/100,R5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="S32">
-        <f>IF($H32="%",S5/100,S5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T32">
-        <f>IF($H32="%",T5/100,T5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U32">
-        <f>IF($H32="%",U5/100,U5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="V32">
-        <f>IF($H32="%",V5/100,V5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="W32">
-        <f>IF($H32="%",W5/100,W5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="X32">
-        <f>IF($H32="%",X5/100,X5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Y32">
-        <f>IF($H32="%",Y5/100,Y5)</f>
+        <f t="shared" si="13"/>
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="Z32">
-        <f>IF($H32="%",Z5/100,Z5)</f>
+        <f t="shared" si="13"/>
         <v>2E-3</v>
       </c>
       <c r="AA32">
-        <f>IF($H32="%",AA5/100,AA5)</f>
+        <f t="shared" si="13"/>
         <v>2E-3</v>
       </c>
       <c r="AB32">
-        <f>IF($H32="%",AB5/100,AB5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AC32">
-        <f>IF($H32="%",AC5/100,AC5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AD32">
-        <f>IF($H32="%",AD5/100,AD5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AE32">
-        <f>IF($H32="%",AE5/100,AE5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF32">
-        <f>IF($H32="%",AF5/100,AF5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AG32">
-        <f>IF($H32="%",AG5/100,AG5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AH32">
-        <f>IF($H32="%",AH5/100,AH5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI32">
-        <f>IF($H32="%",AI5/100,AI5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AJ32">
-        <f>IF($H32="%",AJ5/100,AJ5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
-        <f>B6</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary02</v>
       </c>
       <c r="C33" t="str">
-        <f>C6</f>
+        <f t="shared" si="6"/>
         <v>Sustainable technology R&amp;D</v>
       </c>
       <c r="D33">
-        <f>IF($H6="%",D6*100,D6/12)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E33">
-        <f>IF($H6="%",E6*100,E6/12)</f>
+        <f t="shared" si="11"/>
         <v>33.333333333333329</v>
       </c>
       <c r="F33">
-        <f>IF($H6="%",F6*100,F6/12)</f>
+        <f t="shared" si="11"/>
         <v>50</v>
       </c>
       <c r="G33">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B6,1)))),100,ROUND(G6/12, 1 - _xlfn.CEILING.MATH(LOG10(G6/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H33" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B6,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I33">
-        <f>IF($H33="%",I6/100,I6)</f>
+        <f t="shared" ref="I33:AJ33" si="14">IF($H33="%",I6/100,I6)</f>
         <v>0</v>
       </c>
       <c r="J33">
-        <f>IF($H33="%",J6/100,J6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K33">
-        <f>IF($H33="%",K6/100,K6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L33">
-        <f>IF($H33="%",L6/100,L6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M33">
-        <f>IF($H33="%",M6/100,M6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N33">
-        <f>IF($H33="%",N6/100,N6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O33">
-        <f>IF($H33="%",O6/100,O6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P33">
-        <f>IF($H33="%",P6/100,P6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q33">
-        <f>IF($H33="%",Q6/100,Q6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="R33">
-        <f>IF($H33="%",R6/100,R6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="S33">
-        <f>IF($H33="%",S6/100,S6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="T33">
-        <f>IF($H33="%",T6/100,T6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="U33">
-        <f>IF($H33="%",U6/100,U6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="V33">
-        <f>IF($H33="%",V6/100,V6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="W33">
-        <f>IF($H33="%",W6/100,W6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X33">
-        <f>IF($H33="%",X6/100,X6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y33">
-        <f>IF($H33="%",Y6/100,Y6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Z33">
-        <f>IF($H33="%",Z6/100,Z6)</f>
+        <f t="shared" si="14"/>
         <v>6.9999999999999993E-3</v>
       </c>
       <c r="AA33">
-        <f>IF($H33="%",AA6/100,AA6)</f>
+        <f t="shared" si="14"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AB33">
-        <f>IF($H33="%",AB6/100,AB6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AC33">
-        <f>IF($H33="%",AC6/100,AC6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AD33">
-        <f>IF($H33="%",AD6/100,AD6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AE33">
-        <f>IF($H33="%",AE6/100,AE6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AF33">
-        <f>IF($H33="%",AF6/100,AF6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AG33">
-        <f>IF($H33="%",AG6/100,AG6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH33">
-        <f>IF($H33="%",AH6/100,AH6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AI33">
-        <f>IF($H33="%",AI6/100,AI6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ33">
-        <f>IF($H33="%",AJ6/100,AJ6)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
-        <f>B7</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary2</v>
       </c>
       <c r="C34" t="str">
-        <f>C7</f>
+        <f t="shared" si="6"/>
         <v>Nitrogen and phosphorus cycle</v>
       </c>
       <c r="D34">
-        <f>MIN(D7/($E$2-$E7+D7)*100, 100)</f>
+        <f t="shared" ref="D34:F36" si="15">MIN(D7/($E$2-$E7+D7)*100, 100)</f>
         <v>1.5883253879512418</v>
       </c>
       <c r="E34">
-        <f>MIN(E7/($E$2-$E7+E7)*100, 100)</f>
+        <f t="shared" si="15"/>
         <v>3.1269840936655955</v>
       </c>
       <c r="F34">
-        <f>MIN(F7/($E$2-$E7+F7)*100, 100)</f>
+        <f t="shared" si="15"/>
         <v>9.2118585929110495</v>
       </c>
       <c r="G34">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B7,1)))),100,ROUND(G7/12, 1 - _xlfn.CEILING.MATH(LOG10(G7/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H34" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B7,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I34">
-        <f>IF($H34="%",I7/100,I7)</f>
+        <f t="shared" ref="I34:AJ34" si="16">IF($H34="%",I7/100,I7)</f>
         <v>0</v>
       </c>
       <c r="J34">
-        <f>IF($H34="%",J7/100,J7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K34">
-        <f>IF($H34="%",K7/100,K7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="L34">
-        <f>IF($H34="%",L7/100,L7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M34">
-        <f>IF($H34="%",M7/100,M7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N34">
-        <f>IF($H34="%",N7/100,N7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O34">
-        <f>IF($H34="%",O7/100,O7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P34">
-        <f>IF($H34="%",P7/100,P7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q34">
-        <f>IF($H34="%",Q7/100,Q7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R34">
-        <f>IF($H34="%",R7/100,R7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="S34">
-        <f>IF($H34="%",S7/100,S7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="T34">
-        <f>IF($H34="%",T7/100,T7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="U34">
-        <f>IF($H34="%",U7/100,U7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="V34">
-        <f>IF($H34="%",V7/100,V7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W34">
-        <f>IF($H34="%",W7/100,W7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="X34">
-        <f>IF($H34="%",X7/100,X7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Y34">
-        <f>IF($H34="%",Y7/100,Y7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Z34">
-        <f>IF($H34="%",Z7/100,Z7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AA34">
-        <f>IF($H34="%",AA7/100,AA7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AB34">
-        <f>IF($H34="%",AB7/100,AB7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC34">
-        <f>IF($H34="%",AC7/100,AC7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AD34">
-        <f>IF($H34="%",AD7/100,AD7)</f>
+        <f t="shared" si="16"/>
         <v>2E-3</v>
       </c>
       <c r="AE34">
-        <f>IF($H34="%",AE7/100,AE7)</f>
+        <f t="shared" si="16"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="AF34">
-        <f>IF($H34="%",AF7/100,AF7)</f>
+        <f t="shared" si="16"/>
         <v>1E-3</v>
       </c>
       <c r="AG34">
-        <f>IF($H34="%",AG7/100,AG7)</f>
+        <f t="shared" si="16"/>
         <v>2E-3</v>
       </c>
       <c r="AH34">
-        <f>IF($H34="%",AH7/100,AH7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AI34">
-        <f>IF($H34="%",AI7/100,AI7)</f>
+        <f t="shared" si="16"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="AJ34">
-        <f>IF($H34="%",AJ7/100,AJ7)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
-        <f>B8</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary4</v>
       </c>
       <c r="C35" t="str">
-        <f>C8</f>
+        <f t="shared" si="6"/>
         <v>Freshwater use</v>
       </c>
       <c r="D35">
-        <f>MIN(D8/($E$2-$E8+D8)*100, 100)</f>
+        <f t="shared" si="15"/>
         <v>0.93157420854673556</v>
       </c>
       <c r="E35">
-        <f>MIN(E8/($E$2-$E8+E8)*100, 100)</f>
+        <f t="shared" si="15"/>
         <v>1.8459520043190834</v>
       </c>
       <c r="F35">
-        <f>MIN(F8/($E$2-$E8+F8)*100, 100)</f>
+        <f t="shared" si="15"/>
         <v>3.6249884614771926</v>
       </c>
       <c r="G35">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B8,1)))),100,ROUND(G8/12, 1 - _xlfn.CEILING.MATH(LOG10(G8/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H35" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B8,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I35">
-        <f>IF($H35="%",I8/100,I8)</f>
+        <f t="shared" ref="I35:AJ35" si="17">IF($H35="%",I8/100,I8)</f>
         <v>0</v>
       </c>
       <c r="J35">
-        <f>IF($H35="%",J8/100,J8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K35">
-        <f>IF($H35="%",K8/100,K8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L35">
-        <f>IF($H35="%",L8/100,L8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="M35">
-        <f>IF($H35="%",M8/100,M8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N35">
-        <f>IF($H35="%",N8/100,N8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="O35">
-        <f>IF($H35="%",O8/100,O8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="P35">
-        <f>IF($H35="%",P8/100,P8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Q35">
-        <f>IF($H35="%",Q8/100,Q8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R35">
-        <f>IF($H35="%",R8/100,R8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="S35">
-        <f>IF($H35="%",S8/100,S8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T35">
-        <f>IF($H35="%",T8/100,T8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U35">
-        <f>IF($H35="%",U8/100,U8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="V35">
-        <f>IF($H35="%",V8/100,V8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="W35">
-        <f>IF($H35="%",W8/100,W8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="X35">
-        <f>IF($H35="%",X8/100,X8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Y35">
-        <f>IF($H35="%",Y8/100,Y8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Z35">
-        <f>IF($H35="%",Z8/100,Z8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AA35">
-        <f>IF($H35="%",AA8/100,AA8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AB35">
-        <f>IF($H35="%",AB8/100,AB8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AC35">
-        <f>IF($H35="%",AC8/100,AC8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AD35">
-        <f>IF($H35="%",AD8/100,AD8)</f>
+        <f t="shared" si="17"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AE35">
-        <f>IF($H35="%",AE8/100,AE8)</f>
+        <f t="shared" si="17"/>
         <v>2E-3</v>
       </c>
       <c r="AF35">
-        <f>IF($H35="%",AF8/100,AF8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AG35">
-        <f>IF($H35="%",AG8/100,AG8)</f>
+        <f t="shared" si="17"/>
         <v>1E-3</v>
       </c>
       <c r="AH35">
-        <f>IF($H35="%",AH8/100,AH8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AI35">
-        <f>IF($H35="%",AI8/100,AI8)</f>
+        <f t="shared" si="17"/>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="AJ35">
-        <f>IF($H35="%",AJ8/100,AJ8)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
-        <f>B9</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary5</v>
       </c>
       <c r="C36" t="str">
-        <f>C9</f>
+        <f t="shared" si="6"/>
         <v>Deforestation and other land changes</v>
       </c>
       <c r="D36">
-        <f>MIN(D9/($E$2-$E9+D9)*100, 100)</f>
+        <f t="shared" si="15"/>
         <v>6.6907762735791563</v>
       </c>
       <c r="E36">
-        <f>MIN(E9/($E$2-$E9+E9)*100, 100)</f>
+        <f t="shared" si="15"/>
         <v>15.329500704891871</v>
       </c>
       <c r="F36">
-        <f>MIN(F9/($E$2-$E9+F9)*100, 100)</f>
+        <f t="shared" si="15"/>
         <v>34.493439494279805</v>
       </c>
       <c r="G36">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B9,1)))),100,ROUND(G9/12, 1 - _xlfn.CEILING.MATH(LOG10(G9/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H36" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B9,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I36">
-        <f>IF($H36="%",I9/100,I9)</f>
+        <f t="shared" ref="I36:AJ36" si="18">IF($H36="%",I9/100,I9)</f>
         <v>0.01</v>
       </c>
       <c r="J36">
-        <f>IF($H36="%",J9/100,J9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="K36">
-        <f>IF($H36="%",K9/100,K9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="L36">
-        <f>IF($H36="%",L9/100,L9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="M36">
-        <f>IF($H36="%",M9/100,M9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="N36">
-        <f>IF($H36="%",N9/100,N9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="O36">
-        <f>IF($H36="%",O9/100,O9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="P36">
-        <f>IF($H36="%",P9/100,P9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="Q36">
-        <f>IF($H36="%",Q9/100,Q9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="R36">
-        <f>IF($H36="%",R9/100,R9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="S36">
-        <f>IF($H36="%",S9/100,S9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="T36">
-        <f>IF($H36="%",T9/100,T9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="U36">
-        <f>IF($H36="%",U9/100,U9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="V36">
-        <f>IF($H36="%",V9/100,V9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="W36">
-        <f>IF($H36="%",W9/100,W9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="X36">
-        <f>IF($H36="%",X9/100,X9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="Y36">
-        <f>IF($H36="%",Y9/100,Y9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="Z36">
-        <f>IF($H36="%",Z9/100,Z9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="AA36">
-        <f>IF($H36="%",AA9/100,AA9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="AB36">
-        <f>IF($H36="%",AB9/100,AB9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="AC36">
-        <f>IF($H36="%",AC9/100,AC9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="AD36">
-        <f>IF($H36="%",AD9/100,AD9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="AE36">
-        <f>IF($H36="%",AE9/100,AE9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="AF36">
-        <f>IF($H36="%",AF9/100,AF9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="AG36">
-        <f>IF($H36="%",AG9/100,AG9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="AH36">
-        <f>IF($H36="%",AH9/100,AH9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="AI36">
-        <f>IF($H36="%",AI9/100,AI9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
       <c r="AJ36">
-        <f>IF($H36="%",AJ9/100,AJ9)</f>
+        <f t="shared" si="18"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="37" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
-        <f>B10</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary50</v>
       </c>
       <c r="C37" t="str">
-        <f>C10</f>
+        <f t="shared" si="6"/>
         <v>Primary forest loss</v>
       </c>
       <c r="D37">
-        <f>MIN(D10/($E$9-$E10+D10)*100, 100)</f>
+        <f t="shared" ref="D37:F39" si="19">MIN(D10/($E$9-$E10+D10)*100, 100)</f>
         <v>11.605569163530964</v>
       </c>
       <c r="E37">
-        <f>MIN(E10/($E$9-$E10+E10)*100, 100)</f>
+        <f t="shared" si="19"/>
         <v>23.770078952871572</v>
       </c>
       <c r="F37">
-        <f>MIN(F10/($E$9-$E10+F10)*100, 100)</f>
+        <f t="shared" si="19"/>
         <v>55.50182963669458</v>
       </c>
       <c r="G37">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B10,1)))),100,ROUND(G10/12, 1 - _xlfn.CEILING.MATH(LOG10(G10/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H37" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B10,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I37">
-        <f>IF($H37="%",I10/100,I10)</f>
+        <f t="shared" ref="I37:AJ37" si="20">IF($H37="%",I10/100,I10)</f>
         <v>0</v>
       </c>
       <c r="J37">
-        <f>IF($H37="%",J10/100,J10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="K37">
-        <f>IF($H37="%",K10/100,K10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L37">
-        <f>IF($H37="%",L10/100,L10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M37">
-        <f>IF($H37="%",M10/100,M10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N37">
-        <f>IF($H37="%",N10/100,N10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O37">
-        <f>IF($H37="%",O10/100,O10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="P37">
-        <f>IF($H37="%",P10/100,P10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Q37">
-        <f>IF($H37="%",Q10/100,Q10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R37">
-        <f>IF($H37="%",R10/100,R10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="S37">
-        <f>IF($H37="%",S10/100,S10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="T37">
-        <f>IF($H37="%",T10/100,T10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="U37">
-        <f>IF($H37="%",U10/100,U10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="V37">
-        <f>IF($H37="%",V10/100,V10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="W37">
-        <f>IF($H37="%",W10/100,W10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X37">
-        <f>IF($H37="%",X10/100,X10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Y37">
-        <f>IF($H37="%",Y10/100,Y10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Z37">
-        <f>IF($H37="%",Z10/100,Z10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AA37">
-        <f>IF($H37="%",AA10/100,AA10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AB37">
-        <f>IF($H37="%",AB10/100,AB10)</f>
+        <f t="shared" si="20"/>
         <v>1E-3</v>
       </c>
       <c r="AC37">
-        <f>IF($H37="%",AC10/100,AC10)</f>
+        <f t="shared" si="20"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AD37">
-        <f>IF($H37="%",AD10/100,AD10)</f>
+        <f t="shared" si="20"/>
         <v>1E-3</v>
       </c>
       <c r="AE37">
-        <f>IF($H37="%",AE10/100,AE10)</f>
+        <f t="shared" si="20"/>
         <v>1E-3</v>
       </c>
       <c r="AF37">
-        <f>IF($H37="%",AF10/100,AF10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AG37">
-        <f>IF($H37="%",AG10/100,AG10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AH37">
-        <f>IF($H37="%",AH10/100,AH10)</f>
+        <f t="shared" si="20"/>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="AI37">
-        <f>IF($H37="%",AI10/100,AI10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AJ37">
-        <f>IF($H37="%",AJ10/100,AJ10)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
-        <f>B11</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary51</v>
       </c>
       <c r="C38" t="str">
-        <f>C11</f>
+        <f t="shared" si="6"/>
         <v>Secondary forest loss</v>
       </c>
       <c r="D38">
-        <f>MIN(D11/($E$9-$E11+D11)*100, 100)</f>
+        <f t="shared" si="19"/>
         <v>37.532131949985512</v>
       </c>
       <c r="E38">
-        <f>MIN(E11/($E$9-$E11+E11)*100, 100)</f>
+        <f t="shared" si="19"/>
         <v>54.579437427225116</v>
       </c>
       <c r="F38">
-        <f>MIN(F11/($E$9-$E11+F11)*100, 100)</f>
+        <f t="shared" si="19"/>
         <v>70.6166852922087</v>
       </c>
       <c r="G38">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B11,1)))),100,ROUND(G11/12, 1 - _xlfn.CEILING.MATH(LOG10(G11/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H38" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B11,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I38">
-        <f>IF($H38="%",I11/100,I11)</f>
+        <f t="shared" ref="I38:AJ38" si="21">IF($H38="%",I11/100,I11)</f>
         <v>0</v>
       </c>
       <c r="J38">
-        <f>IF($H38="%",J11/100,J11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K38">
-        <f>IF($H38="%",K11/100,K11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="L38">
-        <f>IF($H38="%",L11/100,L11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="M38">
-        <f>IF($H38="%",M11/100,M11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="N38">
-        <f>IF($H38="%",N11/100,N11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="O38">
-        <f>IF($H38="%",O11/100,O11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="P38">
-        <f>IF($H38="%",P11/100,P11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="Q38">
-        <f>IF($H38="%",Q11/100,Q11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="R38">
-        <f>IF($H38="%",R11/100,R11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S38">
-        <f>IF($H38="%",S11/100,S11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="T38">
-        <f>IF($H38="%",T11/100,T11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="U38">
-        <f>IF($H38="%",U11/100,U11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="V38">
-        <f>IF($H38="%",V11/100,V11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="W38">
-        <f>IF($H38="%",W11/100,W11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="X38">
-        <f>IF($H38="%",X11/100,X11)</f>
+        <f t="shared" si="21"/>
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="Y38">
-        <f>IF($H38="%",Y11/100,Y11)</f>
+        <f t="shared" si="21"/>
         <v>1E-3</v>
       </c>
       <c r="Z38">
-        <f>IF($H38="%",Z11/100,Z11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AA38">
-        <f>IF($H38="%",AA11/100,AA11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AB38">
-        <f>IF($H38="%",AB11/100,AB11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AC38">
-        <f>IF($H38="%",AC11/100,AC11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AD38">
-        <f>IF($H38="%",AD11/100,AD11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AE38">
-        <f>IF($H38="%",AE11/100,AE11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AF38">
-        <f>IF($H38="%",AF11/100,AF11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AG38">
-        <f>IF($H38="%",AG11/100,AG11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AH38">
-        <f>IF($H38="%",AH11/100,AH11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AI38">
-        <f>IF($H38="%",AI11/100,AI11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AJ38">
-        <f>IF($H38="%",AJ11/100,AJ11)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
-        <f>B12</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary52</v>
       </c>
       <c r="C39" t="str">
-        <f>C12</f>
+        <f t="shared" si="6"/>
         <v>Other land changes</v>
       </c>
       <c r="D39">
-        <f>MIN(D12/($E$9-$E12+D12)*100, 100)</f>
+        <f t="shared" si="19"/>
         <v>2.8607306505667411</v>
       </c>
       <c r="E39">
-        <f>MIN(E12/($E$9-$E12+E12)*100, 100)</f>
+        <f t="shared" si="19"/>
         <v>21.650483619903312</v>
       </c>
       <c r="F39">
-        <f>MIN(F12/($E$9-$E12+F12)*100, 100)</f>
+        <f t="shared" si="19"/>
         <v>52.501468782634461</v>
       </c>
       <c r="G39">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B12,1)))),100,ROUND(G12/12, 1 - _xlfn.CEILING.MATH(LOG10(G12/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H39" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B12,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I39">
-        <f>IF($H39="%",I12/100,I12)</f>
+        <f t="shared" ref="I39:AJ39" si="22">IF($H39="%",I12/100,I12)</f>
         <v>0</v>
       </c>
       <c r="J39">
-        <f>IF($H39="%",J12/100,J12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K39">
-        <f>IF($H39="%",K12/100,K12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="L39">
-        <f>IF($H39="%",L12/100,L12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M39">
-        <f>IF($H39="%",M12/100,M12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="N39">
-        <f>IF($H39="%",N12/100,N12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O39">
-        <f>IF($H39="%",O12/100,O12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="P39">
-        <f>IF($H39="%",P12/100,P12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="Q39">
-        <f>IF($H39="%",Q12/100,Q12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="R39">
-        <f>IF($H39="%",R12/100,R12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="S39">
-        <f>IF($H39="%",S12/100,S12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T39">
-        <f>IF($H39="%",T12/100,T12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="U39">
-        <f>IF($H39="%",U12/100,U12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="V39">
-        <f>IF($H39="%",V12/100,V12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W39">
-        <f>IF($H39="%",W12/100,W12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="X39">
-        <f>IF($H39="%",X12/100,X12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="Y39">
-        <f>IF($H39="%",Y12/100,Y12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="Z39">
-        <f>IF($H39="%",Z12/100,Z12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AA39">
-        <f>IF($H39="%",AA12/100,AA12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AB39">
-        <f>IF($H39="%",AB12/100,AB12)</f>
+        <f t="shared" si="22"/>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="AC39">
-        <f>IF($H39="%",AC12/100,AC12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AD39">
-        <f>IF($H39="%",AD12/100,AD12)</f>
+        <f t="shared" si="22"/>
         <v>2E-3</v>
       </c>
       <c r="AE39">
-        <f>IF($H39="%",AE12/100,AE12)</f>
+        <f t="shared" si="22"/>
         <v>2E-3</v>
       </c>
       <c r="AF39">
-        <f>IF($H39="%",AF12/100,AF12)</f>
+        <f t="shared" si="22"/>
         <v>2E-3</v>
       </c>
       <c r="AG39">
-        <f>IF($H39="%",AG12/100,AG12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AH39">
-        <f>IF($H39="%",AH12/100,AH12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AI39">
-        <f>IF($H39="%",AI12/100,AI12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AJ39">
-        <f>IF($H39="%",AJ12/100,AJ12)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
-        <f>B13</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary6</v>
       </c>
       <c r="C40" t="str">
-        <f>C13</f>
+        <f t="shared" si="6"/>
         <v>Biodiversity loss</v>
       </c>
       <c r="D40">
-        <f>MIN(D13/($E$2-$E13+D13)*100, 100)</f>
+        <f t="shared" ref="D40:F41" si="23">MIN(D13/($E$2-$E13+D13)*100, 100)</f>
         <v>0.71891712995873935</v>
       </c>
       <c r="E40">
-        <f>MIN(E13/($E$2-$E13+E13)*100, 100)</f>
+        <f t="shared" si="23"/>
         <v>2.6335789193072028</v>
       </c>
       <c r="F40">
-        <f>MIN(F13/($E$2-$E13+F13)*100, 100)</f>
+        <f t="shared" si="23"/>
         <v>7.5054147182678461</v>
       </c>
       <c r="G40">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B13,1)))),100,ROUND(G13/12, 1 - _xlfn.CEILING.MATH(LOG10(G13/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H40" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B13,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I40">
-        <f>IF($H40="%",I13/100,I13)</f>
+        <f t="shared" ref="I40:AJ40" si="24">IF($H40="%",I13/100,I13)</f>
         <v>0</v>
       </c>
       <c r="J40">
-        <f>IF($H40="%",J13/100,J13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K40">
-        <f>IF($H40="%",K13/100,K13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L40">
-        <f>IF($H40="%",L13/100,L13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M40">
-        <f>IF($H40="%",M13/100,M13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="N40">
-        <f>IF($H40="%",N13/100,N13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O40">
-        <f>IF($H40="%",O13/100,O13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="P40">
-        <f>IF($H40="%",P13/100,P13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q40">
-        <f>IF($H40="%",Q13/100,Q13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="R40">
-        <f>IF($H40="%",R13/100,R13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="S40">
-        <f>IF($H40="%",S13/100,S13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="T40">
-        <f>IF($H40="%",T13/100,T13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="U40">
-        <f>IF($H40="%",U13/100,U13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V40">
-        <f>IF($H40="%",V13/100,V13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="W40">
-        <f>IF($H40="%",W13/100,W13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="X40">
-        <f>IF($H40="%",X13/100,X13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Y40">
-        <f>IF($H40="%",Y13/100,Y13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Z40">
-        <f>IF($H40="%",Z13/100,Z13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AA40">
-        <f>IF($H40="%",AA13/100,AA13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AB40">
-        <f>IF($H40="%",AB13/100,AB13)</f>
+        <f t="shared" si="24"/>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="AC40">
-        <f>IF($H40="%",AC13/100,AC13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AD40">
-        <f>IF($H40="%",AD13/100,AD13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AE40">
-        <f>IF($H40="%",AE13/100,AE13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AF40">
-        <f>IF($H40="%",AF13/100,AF13)</f>
+        <f t="shared" si="24"/>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="AG40">
-        <f>IF($H40="%",AG13/100,AG13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AH40">
-        <f>IF($H40="%",AH13/100,AH13)</f>
+        <f t="shared" si="24"/>
         <v>2E-3</v>
       </c>
       <c r="AI40">
-        <f>IF($H40="%",AI13/100,AI13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AJ40">
-        <f>IF($H40="%",AJ13/100,AJ13)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
-        <f>B14</f>
+        <f t="shared" si="6"/>
         <v>offset-planetary8</v>
       </c>
       <c r="C41" t="str">
-        <f>C14</f>
+        <f t="shared" si="6"/>
         <v>Chemical pollution</v>
       </c>
       <c r="D41">
-        <f>MIN(D14/($E$2-$E14+D14)*100, 100)</f>
+        <f t="shared" si="23"/>
         <v>1.902496914985389</v>
       </c>
       <c r="E41">
-        <f>MIN(E14/($E$2-$E14+E14)*100, 100)</f>
+        <f t="shared" si="23"/>
         <v>5.6785918522750478</v>
       </c>
       <c r="F41">
-        <f>MIN(F14/($E$2-$E14+F14)*100, 100)</f>
+        <f t="shared" si="23"/>
         <v>21.204005162845093</v>
       </c>
       <c r="G41">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B14,1)))),100,ROUND(G14/12, 1 - _xlfn.CEILING.MATH(LOG10(G14/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H41" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B14,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I41">
-        <f>IF($H41="%",I14/100,I14)</f>
+        <f t="shared" ref="I41:AJ41" si="25">IF($H41="%",I14/100,I14)</f>
         <v>0.01</v>
       </c>
       <c r="J41">
-        <f>IF($H41="%",J14/100,J14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="K41">
-        <f>IF($H41="%",K14/100,K14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="L41">
-        <f>IF($H41="%",L14/100,L14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="M41">
-        <f>IF($H41="%",M14/100,M14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="N41">
-        <f>IF($H41="%",N14/100,N14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="O41">
-        <f>IF($H41="%",O14/100,O14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="P41">
-        <f>IF($H41="%",P14/100,P14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="Q41">
-        <f>IF($H41="%",Q14/100,Q14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="R41">
-        <f>IF($H41="%",R14/100,R14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="S41">
-        <f>IF($H41="%",S14/100,S14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="T41">
-        <f>IF($H41="%",T14/100,T14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="U41">
-        <f>IF($H41="%",U14/100,U14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="V41">
-        <f>IF($H41="%",V14/100,V14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="W41">
-        <f>IF($H41="%",W14/100,W14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="X41">
-        <f>IF($H41="%",X14/100,X14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="Y41">
-        <f>IF($H41="%",Y14/100,Y14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="Z41">
-        <f>IF($H41="%",Z14/100,Z14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="AA41">
-        <f>IF($H41="%",AA14/100,AA14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="AB41">
-        <f>IF($H41="%",AB14/100,AB14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="AC41">
-        <f>IF($H41="%",AC14/100,AC14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="AD41">
-        <f>IF($H41="%",AD14/100,AD14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="AE41">
-        <f>IF($H41="%",AE14/100,AE14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="AF41">
-        <f>IF($H41="%",AF14/100,AF14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="AG41">
-        <f>IF($H41="%",AG14/100,AG14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="AH41">
-        <f>IF($H41="%",AH14/100,AH14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="AI41">
-        <f>IF($H41="%",AI14/100,AI14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
       <c r="AJ41">
-        <f>IF($H41="%",AJ14/100,AJ14)</f>
+        <f t="shared" si="25"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="42" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
-        <f t="shared" ref="B42:C42" si="3">B15</f>
+        <f t="shared" ref="B42:C42" si="26">B15</f>
         <v>offset-planetary80</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="26"/>
         <v>Plastics</v>
       </c>
       <c r="D42">
@@ -6222,141 +6223,141 @@
         <v>40.55801156761715</v>
       </c>
       <c r="E42">
-        <f t="shared" ref="E42:F42" si="4">MIN(E15/($E$14-$E15+E15)*100, 100)</f>
+        <f t="shared" ref="E42:F42" si="27">MIN(E15/($E$14-$E15+E15)*100, 100)</f>
         <v>60.013252485788662</v>
       </c>
       <c r="F42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="27"/>
         <v>86.556169429097608</v>
       </c>
       <c r="G42">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B15,1)))),100,ROUND(G15/12, 1 - _xlfn.CEILING.MATH(LOG10(G15/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H42" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B15,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I42">
-        <f t="shared" ref="I42:AI42" si="5">IF($H42="%",I15/100,I15)</f>
+        <f t="shared" ref="I42:AI42" si="28">IF($H42="%",I15/100,I15)</f>
         <v>0</v>
       </c>
       <c r="J42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="L42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="M42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="N42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="P42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="R42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="S42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="T42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="U42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="V42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="W42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="X42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Y42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Z42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AA42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AB42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AC42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AD42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AE42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AF42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AG42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>2E-3</v>
       </c>
       <c r="AH42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AI42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="28"/>
         <v>1E-3</v>
       </c>
       <c r="AJ42">
-        <f t="shared" ref="AJ42" si="6">IF($H42="%",AJ15/100,AJ15)</f>
+        <f t="shared" ref="AJ42" si="29">IF($H42="%",AJ15/100,AJ15)</f>
         <v>6.9999999999999993E-3</v>
       </c>
     </row>
     <row r="43" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
-        <f t="shared" ref="B43:C44" si="7">B16</f>
+        <f t="shared" ref="B43:C44" si="30">B16</f>
         <v>offset-planetary81</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="30"/>
         <v>Persistent organic pollutants</v>
       </c>
       <c r="D43">
@@ -6364,141 +6365,141 @@
         <v>1.3067467529521324</v>
       </c>
       <c r="E43">
-        <f t="shared" ref="E43:F44" si="8">MIN(E16/($E$14-$E16+E16)*100, 100)</f>
+        <f t="shared" ref="E43:F44" si="31">MIN(E16/($E$14-$E16+E16)*100, 100)</f>
         <v>3.4691698756621716</v>
       </c>
       <c r="F43">
+        <f t="shared" si="31"/>
+        <v>6.7057073712508517</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="H43" t="str">
         <f t="shared" si="8"/>
-        <v>6.7057073712508517</v>
-      </c>
-      <c r="G43">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B16,1)))),100,ROUND(G16/12, 1 - _xlfn.CEILING.MATH(LOG10(G16/12))))</f>
-        <v>100</v>
-      </c>
-      <c r="H43" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B16,1))),"$","%")</f>
         <v>%</v>
       </c>
       <c r="I43">
-        <f t="shared" ref="I43:AI44" si="9">IF($H43="%",I16/100,I16)</f>
+        <f t="shared" ref="I43:AI44" si="32">IF($H43="%",I16/100,I16)</f>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="K43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="L43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="S43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="T43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="U43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="W43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="X43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Y43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Z43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AA43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AC43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AD43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AE43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AF43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AG43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AH43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AI43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AJ43">
-        <f t="shared" ref="AJ43:AJ44" si="10">IF($H43="%",AJ16/100,AJ16)</f>
+        <f t="shared" ref="AJ43:AJ44" si="33">IF($H43="%",AJ16/100,AJ16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="30"/>
         <v>offset-planetary81</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="30"/>
         <v>Other pollutants</v>
       </c>
       <c r="D44">
@@ -6506,141 +6507,141 @@
         <v>5.4394911162077548</v>
       </c>
       <c r="E44">
+        <f t="shared" si="31"/>
+        <v>36.517577638549184</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="31"/>
+        <v>74.201510853350641</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="H44" t="str">
         <f t="shared" si="8"/>
-        <v>36.517577638549184</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="8"/>
-        <v>74.201510853350641</v>
-      </c>
-      <c r="G44">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B17,1)))),100,ROUND(G17/12, 1 - _xlfn.CEILING.MATH(LOG10(G17/12))))</f>
-        <v>100</v>
-      </c>
-      <c r="H44" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B17,1))),"$","%")</f>
         <v>%</v>
       </c>
       <c r="I44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="J44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="K44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="L44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="S44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="T44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="U44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="W44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="X44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Y44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="Z44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AA44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AC44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AD44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AE44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AF44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AG44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>6.9999999999999993E-3</v>
       </c>
       <c r="AH44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AI44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="32"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AJ44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
-        <f>B18</f>
+        <f t="shared" ref="B45:C52" si="34">B18</f>
         <v>offset-human</v>
       </c>
       <c r="C45" t="str">
-        <f>C18</f>
+        <f t="shared" si="34"/>
         <v>Human rights violations</v>
       </c>
       <c r="D45">
@@ -6656,133 +6657,133 @@
         <v>16.423926210196189</v>
       </c>
       <c r="G45">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B18,1)))),100,ROUND(G18/12, 1 - _xlfn.CEILING.MATH(LOG10(G18/12))))</f>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="H45" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B18,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>$</v>
       </c>
       <c r="I45">
-        <f>IF($H45="%",I18/100,I18)</f>
+        <f t="shared" ref="I45:AJ45" si="35">IF($H45="%",I18/100,I18)</f>
         <v>1</v>
       </c>
       <c r="J45">
-        <f>IF($H45="%",J18/100,J18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="K45">
-        <f>IF($H45="%",K18/100,K18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="L45">
-        <f>IF($H45="%",L18/100,L18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="M45">
-        <f>IF($H45="%",M18/100,M18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="N45">
-        <f>IF($H45="%",N18/100,N18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="O45">
-        <f>IF($H45="%",O18/100,O18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="P45">
-        <f>IF($H45="%",P18/100,P18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="Q45">
-        <f>IF($H45="%",Q18/100,Q18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="R45">
-        <f>IF($H45="%",R18/100,R18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="S45">
-        <f>IF($H45="%",S18/100,S18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="T45">
-        <f>IF($H45="%",T18/100,T18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="U45">
-        <f>IF($H45="%",U18/100,U18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="V45">
-        <f>IF($H45="%",V18/100,V18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="W45">
-        <f>IF($H45="%",W18/100,W18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="X45">
-        <f>IF($H45="%",X18/100,X18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="Y45">
-        <f>IF($H45="%",Y18/100,Y18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="Z45">
-        <f>IF($H45="%",Z18/100,Z18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="AA45">
-        <f>IF($H45="%",AA18/100,AA18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="AB45">
-        <f>IF($H45="%",AB18/100,AB18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="AC45">
-        <f>IF($H45="%",AC18/100,AC18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="AD45">
-        <f>IF($H45="%",AD18/100,AD18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="AE45">
-        <f>IF($H45="%",AE18/100,AE18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="AF45">
-        <f>IF($H45="%",AF18/100,AF18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="AG45">
-        <f>IF($H45="%",AG18/100,AG18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="AH45">
-        <f>IF($H45="%",AH18/100,AH18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="AI45">
-        <f>IF($H45="%",AI18/100,AI18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="AJ45">
-        <f>IF($H45="%",AJ18/100,AJ18)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
-        <f>B19</f>
+        <f t="shared" si="34"/>
         <v>offset-human0</v>
       </c>
       <c r="C46" t="str">
-        <f>C19</f>
+        <f t="shared" si="34"/>
         <v>Poverty labour</v>
       </c>
       <c r="D46">
@@ -6798,975 +6799,975 @@
         <v>100</v>
       </c>
       <c r="G46">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B19,1)))),100,ROUND(G19/12, 1 - _xlfn.CEILING.MATH(LOG10(G19/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H46" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B19,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I46">
-        <f>IF($H46="%",I19/100,I19)</f>
+        <f t="shared" ref="I46:AJ46" si="36">IF($H46="%",I19/100,I19)</f>
         <v>0.01</v>
       </c>
       <c r="J46">
-        <f>IF($H46="%",J19/100,J19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="K46">
-        <f>IF($H46="%",K19/100,K19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="L46">
-        <f>IF($H46="%",L19/100,L19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="M46">
-        <f>IF($H46="%",M19/100,M19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="N46">
-        <f>IF($H46="%",N19/100,N19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="O46">
-        <f>IF($H46="%",O19/100,O19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="P46">
-        <f>IF($H46="%",P19/100,P19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="Q46">
-        <f>IF($H46="%",Q19/100,Q19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="R46">
-        <f>IF($H46="%",R19/100,R19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="S46">
-        <f>IF($H46="%",S19/100,S19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="T46">
-        <f>IF($H46="%",T19/100,T19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="U46">
-        <f>IF($H46="%",U19/100,U19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="V46">
-        <f>IF($H46="%",V19/100,V19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="W46">
-        <f>IF($H46="%",W19/100,W19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="X46">
-        <f>IF($H46="%",X19/100,X19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="Y46">
-        <f>IF($H46="%",Y19/100,Y19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="Z46">
-        <f>IF($H46="%",Z19/100,Z19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="AA46">
-        <f>IF($H46="%",AA19/100,AA19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="AB46">
-        <f>IF($H46="%",AB19/100,AB19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="AC46">
-        <f>IF($H46="%",AC19/100,AC19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="AD46">
-        <f>IF($H46="%",AD19/100,AD19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="AE46">
-        <f>IF($H46="%",AE19/100,AE19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="AF46">
-        <f>IF($H46="%",AF19/100,AF19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="AG46">
-        <f>IF($H46="%",AG19/100,AG19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="AH46">
-        <f>IF($H46="%",AH19/100,AH19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="AI46">
-        <f>IF($H46="%",AI19/100,AI19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
       <c r="AJ46">
-        <f>IF($H46="%",AJ19/100,AJ19)</f>
+        <f t="shared" si="36"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="47" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
-        <f>B20</f>
+        <f t="shared" si="34"/>
         <v>offset-human00</v>
       </c>
       <c r="C47" t="str">
-        <f>C20</f>
+        <f t="shared" si="34"/>
         <v>Correct country distribution</v>
       </c>
       <c r="D47">
-        <f>IF($H20="%",D20*100,D20/12)</f>
+        <f t="shared" ref="D47:F50" si="37">IF($H20="%",D20*100,D20/12)</f>
         <v>0</v>
       </c>
       <c r="E47">
-        <f>IF($H20="%",E20*100,E20/12)</f>
+        <f t="shared" si="37"/>
         <v>40</v>
       </c>
       <c r="F47">
-        <f>IF($H20="%",F20*100,F20/12)</f>
+        <f t="shared" si="37"/>
         <v>100</v>
       </c>
       <c r="G47">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B20,1)))),100,ROUND(G20/12, 1 - _xlfn.CEILING.MATH(LOG10(G20/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H47" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B20,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I47">
-        <f>IF($H47="%",I20/100,I20)</f>
+        <f t="shared" ref="I47:AJ47" si="38">IF($H47="%",I20/100,I20)</f>
         <v>2.5337837837837845E-4</v>
       </c>
       <c r="J47">
-        <f>IF($H47="%",J20/100,J20)</f>
+        <f t="shared" si="38"/>
         <v>3.3783783783783791E-4</v>
       </c>
       <c r="K47">
-        <f>IF($H47="%",K20/100,K20)</f>
+        <f t="shared" si="38"/>
         <v>1.4358108108108111E-3</v>
       </c>
       <c r="L47">
-        <f>IF($H47="%",L20/100,L20)</f>
+        <f t="shared" si="38"/>
         <v>5.9121621621621625E-4</v>
       </c>
       <c r="M47">
-        <f>IF($H47="%",M20/100,M20)</f>
+        <f t="shared" si="38"/>
         <v>5.4898648648648652E-4</v>
       </c>
       <c r="N47">
-        <f>IF($H47="%",N20/100,N20)</f>
+        <f t="shared" si="38"/>
         <v>1.6891891891891896E-4</v>
       </c>
       <c r="O47">
-        <f>IF($H47="%",O20/100,O20)</f>
+        <f t="shared" si="38"/>
         <v>2.5337837837837845E-4</v>
       </c>
       <c r="P47">
-        <f>IF($H47="%",P20/100,P20)</f>
+        <f t="shared" si="38"/>
         <v>4.2229729729729737E-4</v>
       </c>
       <c r="Q47">
-        <f>IF($H47="%",Q20/100,Q20)</f>
+        <f t="shared" si="38"/>
         <v>1.1824324324324325E-3</v>
       </c>
       <c r="R47">
-        <f>IF($H47="%",R20/100,R20)</f>
+        <f t="shared" si="38"/>
         <v>1.6891891891891896E-4</v>
       </c>
       <c r="S47">
-        <f>IF($H47="%",S20/100,S20)</f>
+        <f t="shared" si="38"/>
         <v>6.7567567567567582E-4</v>
       </c>
       <c r="T47">
-        <f>IF($H47="%",T20/100,T20)</f>
+        <f t="shared" si="38"/>
         <v>1.5625000000000003E-3</v>
       </c>
       <c r="U47">
-        <f>IF($H47="%",U20/100,U20)</f>
+        <f t="shared" si="38"/>
         <v>1.5625000000000003E-3</v>
       </c>
       <c r="V47">
-        <f>IF($H47="%",V20/100,V20)</f>
+        <f t="shared" si="38"/>
         <v>5.9121621621621625E-4</v>
       </c>
       <c r="W47">
-        <f>IF($H47="%",W20/100,W20)</f>
+        <f t="shared" si="38"/>
         <v>2.4493243243243248E-4</v>
       </c>
       <c r="X47">
-        <f>IF($H47="%",X20/100,X20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Y47">
-        <f>IF($H47="%",Y20/100,Y20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Z47">
-        <f>IF($H47="%",Z20/100,Z20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AA47">
-        <f>IF($H47="%",AA20/100,AA20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB47">
-        <f>IF($H47="%",AB20/100,AB20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AC47">
-        <f>IF($H47="%",AC20/100,AC20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AD47">
-        <f>IF($H47="%",AD20/100,AD20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AE47">
-        <f>IF($H47="%",AE20/100,AE20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AF47">
-        <f>IF($H47="%",AF20/100,AF20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AG47">
-        <f>IF($H47="%",AG20/100,AG20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AH47">
-        <f>IF($H47="%",AH20/100,AH20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AI47">
-        <f>IF($H47="%",AI20/100,AI20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AJ47">
-        <f>IF($H47="%",AJ20/100,AJ20)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
-        <f>B21</f>
+        <f t="shared" si="34"/>
         <v>offset-human01</v>
       </c>
       <c r="C48" t="str">
-        <f>C21</f>
+        <f t="shared" si="34"/>
         <v>Most needing people</v>
       </c>
       <c r="D48">
-        <f>IF($H21="%",D21*100,D21/12)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="E48">
-        <f>IF($H21="%",E21*100,E21/12)</f>
+        <f t="shared" si="37"/>
         <v>40</v>
       </c>
       <c r="F48">
-        <f>IF($H21="%",F21*100,F21/12)</f>
+        <f t="shared" si="37"/>
         <v>100</v>
       </c>
       <c r="G48">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B21,1)))),100,ROUND(G21/12, 1 - _xlfn.CEILING.MATH(LOG10(G21/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H48" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B21,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I48">
-        <f>IF($H48="%",I21/100,I21)</f>
+        <f t="shared" ref="I48:AJ48" si="39">IF($H48="%",I21/100,I21)</f>
         <v>9.0909090999999993E-4</v>
       </c>
       <c r="J48">
-        <f>IF($H48="%",J21/100,J21)</f>
+        <f t="shared" si="39"/>
         <v>9.0909090999999993E-4</v>
       </c>
       <c r="K48">
-        <f>IF($H48="%",K21/100,K21)</f>
+        <f t="shared" si="39"/>
         <v>9.0909090999999993E-4</v>
       </c>
       <c r="L48">
-        <f>IF($H48="%",L21/100,L21)</f>
+        <f t="shared" si="39"/>
         <v>9.0909090999999993E-4</v>
       </c>
       <c r="M48">
-        <f>IF($H48="%",M21/100,M21)</f>
+        <f t="shared" si="39"/>
         <v>9.0909090999999993E-4</v>
       </c>
       <c r="N48">
-        <f>IF($H48="%",N21/100,N21)</f>
+        <f t="shared" si="39"/>
         <v>9.0909090999999993E-4</v>
       </c>
       <c r="O48">
-        <f>IF($H48="%",O21/100,O21)</f>
+        <f t="shared" si="39"/>
         <v>9.0909090999999993E-4</v>
       </c>
       <c r="P48">
-        <f>IF($H48="%",P21/100,P21)</f>
+        <f t="shared" si="39"/>
         <v>9.0909090999999993E-4</v>
       </c>
       <c r="Q48">
-        <f>IF($H48="%",Q21/100,Q21)</f>
+        <f t="shared" si="39"/>
         <v>9.0909090999999993E-4</v>
       </c>
       <c r="R48">
-        <f>IF($H48="%",R21/100,R21)</f>
+        <f t="shared" si="39"/>
         <v>9.0909090999999993E-4</v>
       </c>
       <c r="S48">
-        <f>IF($H48="%",S21/100,S21)</f>
+        <f t="shared" si="39"/>
         <v>9.0909090999999993E-4</v>
       </c>
       <c r="T48">
-        <f>IF($H48="%",T21/100,T21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="U48">
-        <f>IF($H48="%",U21/100,U21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="V48">
-        <f>IF($H48="%",V21/100,V21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="W48">
-        <f>IF($H48="%",W21/100,W21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X48">
-        <f>IF($H48="%",X21/100,X21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y48">
-        <f>IF($H48="%",Y21/100,Y21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Z48">
-        <f>IF($H48="%",Z21/100,Z21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA48">
-        <f>IF($H48="%",AA21/100,AA21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AB48">
-        <f>IF($H48="%",AB21/100,AB21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AC48">
-        <f>IF($H48="%",AC21/100,AC21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AD48">
-        <f>IF($H48="%",AD21/100,AD21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AE48">
-        <f>IF($H48="%",AE21/100,AE21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AF48">
-        <f>IF($H48="%",AF21/100,AF21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AG48">
-        <f>IF($H48="%",AG21/100,AG21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AH48">
-        <f>IF($H48="%",AH21/100,AH21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AI48">
-        <f>IF($H48="%",AI21/100,AI21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AJ48">
-        <f>IF($H48="%",AJ21/100,AJ21)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
-        <f>B22</f>
+        <f t="shared" si="34"/>
         <v>offset-human02</v>
       </c>
       <c r="C49" t="str">
-        <f>C22</f>
+        <f t="shared" si="34"/>
         <v>Direct donations</v>
       </c>
       <c r="D49">
-        <f>IF($H22="%",D22*100,D22/12)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="E49">
-        <f>IF($H22="%",E22*100,E22/12)</f>
+        <f t="shared" si="37"/>
         <v>20</v>
       </c>
       <c r="F49">
-        <f>IF($H22="%",F22*100,F22/12)</f>
+        <f t="shared" si="37"/>
         <v>100</v>
       </c>
       <c r="G49">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B22,1)))),100,ROUND(G22/12, 1 - _xlfn.CEILING.MATH(LOG10(G22/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H49" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B22,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I49">
-        <f>IF($H49="%",I22/100,I22)</f>
+        <f t="shared" ref="I49:AJ49" si="40">IF($H49="%",I22/100,I22)</f>
         <v>0</v>
       </c>
       <c r="J49">
-        <f>IF($H49="%",J22/100,J22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K49">
-        <f>IF($H49="%",K22/100,K22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="L49">
-        <f>IF($H49="%",L22/100,L22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="M49">
-        <f>IF($H49="%",M22/100,M22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="N49">
-        <f>IF($H49="%",N22/100,N22)</f>
+        <f t="shared" si="40"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="O49">
-        <f>IF($H49="%",O22/100,O22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="P49">
-        <f>IF($H49="%",P22/100,P22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Q49">
-        <f>IF($H49="%",Q22/100,Q22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="R49">
-        <f>IF($H49="%",R22/100,R22)</f>
+        <f t="shared" si="40"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="S49">
-        <f>IF($H49="%",S22/100,S22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="T49">
-        <f>IF($H49="%",T22/100,T22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="U49">
-        <f>IF($H49="%",U22/100,U22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="V49">
-        <f>IF($H49="%",V22/100,V22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W49">
-        <f>IF($H49="%",W22/100,W22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="X49">
-        <f>IF($H49="%",X22/100,X22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Y49">
-        <f>IF($H49="%",Y22/100,Y22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Z49">
-        <f>IF($H49="%",Z22/100,Z22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AA49">
-        <f>IF($H49="%",AA22/100,AA22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AB49">
-        <f>IF($H49="%",AB22/100,AB22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AC49">
-        <f>IF($H49="%",AC22/100,AC22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AD49">
-        <f>IF($H49="%",AD22/100,AD22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AE49">
-        <f>IF($H49="%",AE22/100,AE22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AF49">
-        <f>IF($H49="%",AF22/100,AF22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AG49">
-        <f>IF($H49="%",AG22/100,AG22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AH49">
-        <f>IF($H49="%",AH22/100,AH22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AI49">
-        <f>IF($H49="%",AI22/100,AI22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AJ49">
-        <f>IF($H49="%",AJ22/100,AJ22)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
-        <f>B23</f>
+        <f t="shared" si="34"/>
         <v>offset-animal</v>
       </c>
       <c r="C50" t="str">
-        <f>C23</f>
+        <f t="shared" si="34"/>
         <v>Animal welfare damage</v>
       </c>
       <c r="D50">
-        <f>IF($H23="%",D23*100,D23/12)</f>
-        <v>4.1666666666666664E-2</v>
+        <f t="shared" si="37"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="E50">
-        <f>IF($H23="%",E23*100,E23/12)</f>
-        <v>8.3333333333333329E-2</v>
+        <f t="shared" si="37"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F50">
-        <f>IF($H23="%",F23*100,F23/12)</f>
-        <v>0.83333333333333337</v>
+        <f t="shared" si="37"/>
+        <v>1.6666666666666667</v>
       </c>
       <c r="G50">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B23,1)))),100,ROUND(G23/12, 1 - _xlfn.CEILING.MATH(LOG10(G23/12))))</f>
-        <v>4</v>
+        <f t="shared" si="7"/>
+        <v>3</v>
       </c>
       <c r="H50" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B23,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>$</v>
       </c>
       <c r="I50">
-        <f>IF($H50="%",I23/100,I23)</f>
+        <f t="shared" ref="I50:AJ50" si="41">IF($H50="%",I23/100,I23)</f>
         <v>1</v>
       </c>
       <c r="J50">
-        <f>IF($H50="%",J23/100,J23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="K50">
-        <f>IF($H50="%",K23/100,K23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="L50">
-        <f>IF($H50="%",L23/100,L23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="M50">
-        <f>IF($H50="%",M23/100,M23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="N50">
-        <f>IF($H50="%",N23/100,N23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="O50">
-        <f>IF($H50="%",O23/100,O23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="P50">
-        <f>IF($H50="%",P23/100,P23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="Q50">
-        <f>IF($H50="%",Q23/100,Q23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="R50">
-        <f>IF($H50="%",R23/100,R23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="S50">
-        <f>IF($H50="%",S23/100,S23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="T50">
-        <f>IF($H50="%",T23/100,T23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="U50">
-        <f>IF($H50="%",U23/100,U23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="V50">
-        <f>IF($H50="%",V23/100,V23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="W50">
-        <f>IF($H50="%",W23/100,W23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="X50">
-        <f>IF($H50="%",X23/100,X23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="Y50">
-        <f>IF($H50="%",Y23/100,Y23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="Z50">
-        <f>IF($H50="%",Z23/100,Z23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="AA50">
-        <f>IF($H50="%",AA23/100,AA23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="AB50">
-        <f>IF($H50="%",AB23/100,AB23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="AC50">
-        <f>IF($H50="%",AC23/100,AC23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="AD50">
-        <f>IF($H50="%",AD23/100,AD23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="AE50">
-        <f>IF($H50="%",AE23/100,AE23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="AF50">
-        <f>IF($H50="%",AF23/100,AF23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="AG50">
-        <f>IF($H50="%",AG23/100,AG23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="AH50">
-        <f>IF($H50="%",AH23/100,AH23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="AI50">
-        <f>IF($H50="%",AI23/100,AI23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="AJ50">
-        <f>IF($H50="%",AJ23/100,AJ23)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
-        <f>B24</f>
+        <f t="shared" si="34"/>
         <v>offset-animal0</v>
       </c>
       <c r="C51" t="str">
-        <f>C24</f>
+        <f t="shared" si="34"/>
         <v>Wildlife</v>
       </c>
       <c r="D51">
-        <f>MIN(D24/($E$23-$E24+D24)*100, 100)</f>
-        <v>0</v>
+        <f t="shared" ref="D51:F52" si="42">MIN(D24/($E$23-$E24+D24)*100, 100)</f>
+        <v>33.333333333333329</v>
       </c>
       <c r="E51">
-        <f>MIN(E24/($E$23-$E24+E24)*100, 100)</f>
-        <v>0</v>
+        <f t="shared" si="42"/>
+        <v>50</v>
       </c>
       <c r="F51">
-        <f>MIN(F24/($E$23-$E24+F24)*100, 100)</f>
-        <v>0</v>
+        <f t="shared" si="42"/>
+        <v>90.909090909090907</v>
       </c>
       <c r="G51">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B24,1)))),100,ROUND(G24/12, 1 - _xlfn.CEILING.MATH(LOG10(G24/12))))</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="H51" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B24,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I51">
-        <f>IF($H51="%",I24/100,I24)</f>
+        <f t="shared" ref="I51:AJ51" si="43">IF($H51="%",I24/100,I24)</f>
         <v>0</v>
       </c>
       <c r="J51">
-        <f>IF($H51="%",J24/100,J24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="K51">
-        <f>IF($H51="%",K24/100,K24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="L51">
-        <f>IF($H51="%",L24/100,L24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="M51">
-        <f>IF($H51="%",M24/100,M24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="N51">
-        <f>IF($H51="%",N24/100,N24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="O51">
-        <f>IF($H51="%",O24/100,O24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="P51">
-        <f>IF($H51="%",P24/100,P24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q51">
-        <f>IF($H51="%",Q24/100,Q24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="R51">
-        <f>IF($H51="%",R24/100,R24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="S51">
-        <f>IF($H51="%",S24/100,S24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="T51">
-        <f>IF($H51="%",T24/100,T24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="U51">
-        <f>IF($H51="%",U24/100,U24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="V51">
-        <f>IF($H51="%",V24/100,V24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="W51">
-        <f>IF($H51="%",W24/100,W24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="X51">
-        <f>IF($H51="%",X24/100,X24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Y51">
-        <f>IF($H51="%",Y24/100,Y24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Z51">
-        <f>IF($H51="%",Z24/100,Z24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AA51">
-        <f>IF($H51="%",AA24/100,AA24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AB51">
-        <f>IF($H51="%",AB24/100,AB24)</f>
+        <f t="shared" si="43"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AC51">
-        <f>IF($H51="%",AC24/100,AC24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AD51">
-        <f>IF($H51="%",AD24/100,AD24)</f>
+        <f t="shared" si="43"/>
         <v>1E-3</v>
       </c>
       <c r="AE51">
-        <f>IF($H51="%",AE24/100,AE24)</f>
+        <f t="shared" si="43"/>
         <v>1E-3</v>
       </c>
       <c r="AF51">
-        <f>IF($H51="%",AF24/100,AF24)</f>
+        <f t="shared" si="43"/>
         <v>2E-3</v>
       </c>
       <c r="AG51">
-        <f>IF($H51="%",AG24/100,AG24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AH51">
-        <f>IF($H51="%",AH24/100,AH24)</f>
+        <f t="shared" si="43"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AI51">
-        <f>IF($H51="%",AI24/100,AI24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="AJ51">
-        <f>IF($H51="%",AJ24/100,AJ24)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
-        <f>B25</f>
+        <f t="shared" si="34"/>
         <v>offset-animal1</v>
       </c>
       <c r="C52" t="str">
-        <f>C25</f>
+        <f t="shared" si="34"/>
         <v>Farm animals</v>
       </c>
       <c r="D52">
-        <f>MIN(D25/($E$23-$E25+D25)*100, 100)</f>
+        <f t="shared" si="42"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="42"/>
+        <v>50</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="42"/>
+        <v>90.909090909090907</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
-      <c r="E52">
-        <f>MIN(E25/($E$23-$E25+E25)*100, 100)</f>
-        <v>100</v>
-      </c>
-      <c r="F52">
-        <f>MIN(F25/($E$23-$E25+F25)*100, 100)</f>
-        <v>100</v>
-      </c>
-      <c r="G52">
-        <f>IF(NOT(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B25,1)))),100,ROUND(G25/12, 1 - _xlfn.CEILING.MATH(LOG10(G25/12))))</f>
-        <v>100</v>
-      </c>
       <c r="H52" t="str">
-        <f>IF(ISERROR(_xlfn.NUMBERVALUE(RIGHT(B25,1))),"$","%")</f>
+        <f t="shared" si="8"/>
         <v>%</v>
       </c>
       <c r="I52">
-        <f>IF($H52="%",I25/100,I25)</f>
+        <f t="shared" ref="I52:AJ52" si="44">IF($H52="%",I25/100,I25)</f>
         <v>0</v>
       </c>
       <c r="J52">
-        <f>IF($H52="%",J25/100,J25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="K52">
-        <f>IF($H52="%",K25/100,K25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="L52">
-        <f>IF($H52="%",L25/100,L25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="M52">
-        <f>IF($H52="%",M25/100,M25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="N52">
-        <f>IF($H52="%",N25/100,N25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="O52">
-        <f>IF($H52="%",O25/100,O25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="P52">
-        <f>IF($H52="%",P25/100,P25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="Q52">
-        <f>IF($H52="%",Q25/100,Q25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="R52">
-        <f>IF($H52="%",R25/100,R25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="S52">
-        <f>IF($H52="%",S25/100,S25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="T52">
-        <f>IF($H52="%",T25/100,T25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="U52">
-        <f>IF($H52="%",U25/100,U25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="V52">
-        <f>IF($H52="%",V25/100,V25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="W52">
-        <f>IF($H52="%",W25/100,W25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="X52">
-        <f>IF($H52="%",X25/100,X25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="Y52">
-        <f>IF($H52="%",Y25/100,Y25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="Z52">
-        <f>IF($H52="%",Z25/100,Z25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AA52">
-        <f>IF($H52="%",AA25/100,AA25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AB52">
-        <f>IF($H52="%",AB25/100,AB25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AC52">
-        <f>IF($H52="%",AC25/100,AC25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AD52">
-        <f>IF($H52="%",AD25/100,AD25)</f>
+        <f t="shared" si="44"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AE52">
-        <f>IF($H52="%",AE25/100,AE25)</f>
+        <f t="shared" si="44"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AF52">
-        <f>IF($H52="%",AF25/100,AF25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AG52">
-        <f>IF($H52="%",AG25/100,AG25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AH52">
-        <f>IF($H52="%",AH25/100,AH25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AI52">
-        <f>IF($H52="%",AI25/100,AI25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="AJ52">
-        <f>IF($H52="%",AJ25/100,AJ25)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -54201,16 +54202,16 @@
         <v>Animal welfare damage</v>
       </c>
       <c r="F23">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I23">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J23" t="str">
         <v>£</v>
@@ -56309,16 +56310,16 @@
         <v>Wildlife</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="J24" t="str">
         <v>£</v>
@@ -58426,7 +58427,7 @@
         <v>10</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="J25" t="str">
         <v>£</v>

</xml_diff>

<commit_message>
fixed donation calculations, wip on fixing slider interactions
</commit_message>
<xml_diff>
--- a/calculations/master_spreadsheet.xlsx
+++ b/calculations/master_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sucha\programming\offset_me\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5C2806-2CC5-42A7-8E2D-DCC2DB49C352}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB3E3EE-3E8B-4B10-900F-7500531283AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="payments" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -1384,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E8D887-92D5-48D4-A2E3-CF1AF56E27C5}">
   <dimension ref="A1:AJ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C20:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7784,8 +7784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254106CF-5557-4B21-A947-723F3A530508}">
   <dimension ref="A1:AAB25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47880,6 +47880,9 @@
       <c r="B20" t="s">
         <v>93</v>
       </c>
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
       <c r="E20" t="str">
         <v>Correct country distribution</v>
       </c>
@@ -49988,6 +49991,9 @@
       <c r="B21" t="s">
         <v>93</v>
       </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
       <c r="E21" t="str">
         <v>Most needing people</v>
       </c>
@@ -52095,6 +52101,9 @@
       </c>
       <c r="B22" t="s">
         <v>93</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
       </c>
       <c r="E22" t="str">
         <v>Direct donations</v>

</xml_diff>